<commit_message>
Made the rules dynamic- Added another page 'rules.html' for viewing, adding, updating, and deleting rules. Uses PostgreSQL database for storing the rules.
</commit_message>
<xml_diff>
--- a/sample_transactions_new.xlsx
+++ b/sample_transactions_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kpmg\fraud-detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872EF455-8216-41E2-83E1-C3E8B5BA2A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1912A20-2FD3-4531-8DE8-442318D63CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>